<commit_message>
vector2/3d added + bug fix
</commit_message>
<xml_diff>
--- a/matrix_multiplication_example.xlsx
+++ b/matrix_multiplication_example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositories\Avans\Minor\LINAL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C9E5844A-CDC4-450E-8B8B-E4F57BEB2683}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DBDB48C-46BD-4E87-93FB-5BECB89F95D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F95EB617-4C15-40B8-83E0-75A4B6C95CDB}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F95EB617-4C15-40B8-83E0-75A4B6C95CDB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="10">
   <si>
     <t>row</t>
   </si>
@@ -61,6 +61,9 @@
   </si>
   <si>
     <t>[3 * 3]</t>
+  </si>
+  <si>
+    <t>*</t>
   </si>
 </sst>
 </file>
@@ -450,17 +453,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25E51DF5-73A4-4900-BF25-C15BDB9DEB8F}">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -646,9 +651,11 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
+      <c r="B13" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="C13" s="1" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>5</v>

</xml_diff>